<commit_message>
feat: redesign game_06 skill tree
</commit_message>
<xml_diff>
--- a/example/game_06_abyssal_nightfall/skill_tree.xlsx
+++ b/example/game_06_abyssal_nightfall/skill_tree.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A4:K14"/>
+  <dimension ref="A4:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -483,10 +483,10 @@
         <v>0001</v>
       </c>
       <c r="D6" t="str">
-        <v>聚焦锚点</v>
+        <v>裂变弹匣</v>
       </c>
       <c r="E6" t="str">
-        <v>精准</v>
+        <v>弹道</v>
       </c>
       <c r="F6" t="str">
         <v>1</v>
@@ -495,13 +495,13 @@
         <v/>
       </c>
       <c r="H6" t="str">
-        <v>暴击:+5|稳定:+8</v>
+        <v>split:+1|splitAngle:+12|damage:+6</v>
       </c>
       <c r="I6" t="str">
         <v>level:3</v>
       </c>
       <c r="J6" t="str">
-        <v>提高命中稳定，解锁精准分支。</v>
+        <v>将弹道裂变为额外子弹，基础火力提升。</v>
       </c>
       <c r="K6" t="str">
         <v>icons/skill/focal_anchor.png</v>
@@ -518,10 +518,10 @@
         <v>0002</v>
       </c>
       <c r="D7" t="str">
-        <v>极速虹吸</v>
+        <v>轨迹稳流</v>
       </c>
       <c r="E7" t="str">
-        <v>精准</v>
+        <v>弹道</v>
       </c>
       <c r="F7" t="str">
         <v>2</v>
@@ -530,13 +530,13 @@
         <v>skill:70010001</v>
       </c>
       <c r="H7" t="str">
-        <v>装填:-6%|暴击:+4</v>
+        <v>stability:+14|projectileSize:+18|projectileSpeed:+8</v>
       </c>
       <c r="I7" t="str">
         <v>level:6</v>
       </c>
       <c r="J7" t="str">
-        <v>装填更迅速并提升暴击。</v>
+        <v>导流装置压制散布，并扩大弹道厚度。</v>
       </c>
       <c r="K7" t="str">
         <v>icons/skill/rapid_siphon.png</v>
@@ -553,10 +553,10 @@
         <v>0003</v>
       </c>
       <c r="D8" t="str">
-        <v>零点穿透</v>
+        <v>深域贯穿</v>
       </c>
       <c r="E8" t="str">
-        <v>精准</v>
+        <v>弹道</v>
       </c>
       <c r="F8" t="str">
         <v>3</v>
@@ -565,13 +565,13 @@
         <v>skill:70010002</v>
       </c>
       <c r="H8" t="str">
-        <v>伤害:+12|弱点:+20%</v>
+        <v>pierce:+2|crit:+5|damage:+10</v>
       </c>
       <c r="I8" t="str">
         <v>level:9</v>
       </c>
       <c r="J8" t="str">
-        <v>子弹穿透时获得额外伤害。</v>
+        <v>强化穿甲结构并提升暴击输出。</v>
       </c>
       <c r="K8" t="str">
         <v>icons/skill/zero_point.png</v>
@@ -588,10 +588,10 @@
         <v>0001</v>
       </c>
       <c r="D9" t="str">
-        <v>以太共振</v>
+        <v>棱镜导光</v>
       </c>
       <c r="E9" t="str">
-        <v>以太</v>
+        <v>能量</v>
       </c>
       <c r="F9" t="str">
         <v>1</v>
@@ -600,13 +600,13 @@
         <v/>
       </c>
       <c r="H9" t="str">
-        <v>光束伤害:+6|理智消耗:-2</v>
+        <v>damage:+6|sanityDrain:-6|projectileSize:+18</v>
       </c>
       <c r="I9" t="str">
-        <v>level:4</v>
+        <v>level:4|weaponAttack:BEAM</v>
       </c>
       <c r="J9" t="str">
-        <v>持续型武器效率提升。</v>
+        <v>棱镜束缚能量消耗，同时扩大光束宽度。</v>
       </c>
       <c r="K9" t="str">
         <v>icons/skill/aether_resonance.png</v>
@@ -623,10 +623,10 @@
         <v>0002</v>
       </c>
       <c r="D10" t="str">
-        <v>合唱激流</v>
+        <v>谐振折叠</v>
       </c>
       <c r="E10" t="str">
-        <v>以太</v>
+        <v>能量</v>
       </c>
       <c r="F10" t="str">
         <v>2</v>
@@ -635,13 +635,13 @@
         <v>skill:70020001</v>
       </c>
       <c r="H10" t="str">
-        <v>蓄力:+4/s|半径:+0.8</v>
+        <v>damageMultiplier:+8|projectileSpeed:+14|stability:+8</v>
       </c>
       <c r="I10" t="str">
-        <v>level:7</v>
+        <v>level:7|weaponAttack:BEAM</v>
       </c>
       <c r="J10" t="str">
-        <v>光束蓄力更快并扩大范围。</v>
+        <v>折叠振镜提高能量聚焦与射速。</v>
       </c>
       <c r="K10" t="str">
         <v>icons/skill/choir_surge.png</v>
@@ -652,34 +652,34 @@
         <v>70</v>
       </c>
       <c r="B11" t="str">
-        <v>03</v>
+        <v>02</v>
       </c>
       <c r="C11" t="str">
-        <v>0001</v>
+        <v>0003</v>
       </c>
       <c r="D11" t="str">
-        <v>回涌之握</v>
+        <v>相干放射</v>
       </c>
       <c r="E11" t="str">
-        <v>潮汐</v>
+        <v>能量</v>
       </c>
       <c r="F11" t="str">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G11" t="str">
-        <v/>
+        <v>skill:70020002</v>
       </c>
       <c r="H11" t="str">
-        <v>牵引:+18|霜寒伤害:+10</v>
+        <v>ricochet:+1|crit:+6|damage:+12</v>
       </c>
       <c r="I11" t="str">
-        <v>level:5</v>
+        <v>level:10|weaponAttack:BEAM</v>
       </c>
       <c r="J11" t="str">
-        <v>潮汐技能增强牵引力。</v>
+        <v>相干腔反复震荡，使光束可在敌间折射。</v>
       </c>
       <c r="K11" t="str">
-        <v>icons/skill/undertow.png</v>
+        <v>icons/skill/zero_point.png</v>
       </c>
     </row>
     <row r="12">
@@ -690,31 +690,31 @@
         <v>03</v>
       </c>
       <c r="C12" t="str">
-        <v>0002</v>
+        <v>0001</v>
       </c>
       <c r="D12" t="str">
-        <v>裂潮坠落</v>
+        <v>相位壁垒</v>
       </c>
       <c r="E12" t="str">
-        <v>潮汐</v>
+        <v>护卫</v>
       </c>
       <c r="F12" t="str">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G12" t="str">
-        <v>skill:70030001</v>
+        <v/>
       </c>
       <c r="H12" t="str">
-        <v>霜裂:+22|范围:+1.2</v>
+        <v>shield:+60|contactResist:+25|sanityRegen:+3</v>
       </c>
       <c r="I12" t="str">
-        <v>level:8</v>
+        <v>level:4</v>
       </c>
       <c r="J12" t="str">
-        <v>爆裂范围扩大并追加寒霜伤害。</v>
+        <v>展开相位护壁，降低接触伤害并补充理智。</v>
       </c>
       <c r="K12" t="str">
-        <v>icons/skill/riptide_collapse.png</v>
+        <v>icons/skill/ward_bastion.png</v>
       </c>
     </row>
     <row r="13">
@@ -722,34 +722,34 @@
         <v>70</v>
       </c>
       <c r="B13" t="str">
-        <v>04</v>
+        <v>03</v>
       </c>
       <c r="C13" t="str">
-        <v>0001</v>
+        <v>0002</v>
       </c>
       <c r="D13" t="str">
-        <v>护域壁垒</v>
+        <v>护盾崩击</v>
       </c>
       <c r="E13" t="str">
-        <v>守御</v>
+        <v>护卫</v>
       </c>
       <c r="F13" t="str">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G13" t="str">
-        <v/>
+        <v>skill:70030001</v>
       </c>
       <c r="H13" t="str">
-        <v>护盾:+40|理智恢复:+3</v>
+        <v>meleeDamage:+70|meleeRadius:+20|meleeInterval:-0.5</v>
       </c>
       <c r="I13" t="str">
-        <v>level:4</v>
+        <v>level:7</v>
       </c>
       <c r="J13" t="str">
-        <v>短期内提高护盾与理智恢复。</v>
+        <v>护盾冲击形成短距爆发，持续清理近身威胁。</v>
       </c>
       <c r="K13" t="str">
-        <v>icons/skill/ward_bastion.png</v>
+        <v>icons/skill/seraphic_shell.png</v>
       </c>
     </row>
     <row r="14">
@@ -757,39 +757,144 @@
         <v>70</v>
       </c>
       <c r="B14" t="str">
+        <v>03</v>
+      </c>
+      <c r="C14" t="str">
+        <v>0003</v>
+      </c>
+      <c r="D14" t="str">
+        <v>寂光回响</v>
+      </c>
+      <c r="E14" t="str">
+        <v>护卫</v>
+      </c>
+      <c r="F14" t="str">
+        <v>3</v>
+      </c>
+      <c r="G14" t="str">
+        <v>skill:70030002</v>
+      </c>
+      <c r="H14" t="str">
+        <v>beamReflect:20%|shieldRegen:+16|invulnTime:+0.4</v>
+      </c>
+      <c r="I14" t="str">
+        <v>level:10</v>
+      </c>
+      <c r="J14" t="str">
+        <v>护盾折射寂光，可短暂反弹能量。</v>
+      </c>
+      <c r="K14" t="str">
+        <v>icons/skill/ward_bastion.png</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>70</v>
+      </c>
+      <c r="B15" t="str">
         <v>04</v>
       </c>
-      <c r="C14" t="str">
+      <c r="C15" t="str">
+        <v>0001</v>
+      </c>
+      <c r="D15" t="str">
+        <v>术式镀层</v>
+      </c>
+      <c r="E15" t="str">
+        <v>工坊</v>
+      </c>
+      <c r="F15" t="str">
+        <v>1</v>
+      </c>
+      <c r="G15" t="str">
+        <v/>
+      </c>
+      <c r="H15" t="str">
+        <v>projectileSize:+24|elementSlow:+18|elementSlowDuration:+1.4</v>
+      </c>
+      <c r="I15" t="str">
+        <v>level:5</v>
+      </c>
+      <c r="J15" t="str">
+        <v>在弹体上刻蚀术式，对命中目标施加霜蚀减速。</v>
+      </c>
+      <c r="K15" t="str">
+        <v>icons/skill/undertow.png</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>70</v>
+      </c>
+      <c r="B16" t="str">
+        <v>04</v>
+      </c>
+      <c r="C16" t="str">
         <v>0002</v>
       </c>
-      <c r="D14" t="str">
-        <v>炽天护壳</v>
-      </c>
-      <c r="E14" t="str">
-        <v>守御</v>
-      </c>
-      <c r="F14" t="str">
+      <c r="D16" t="str">
+        <v>弹道精铸</v>
+      </c>
+      <c r="E16" t="str">
+        <v>工坊</v>
+      </c>
+      <c r="F16" t="str">
         <v>2</v>
       </c>
-      <c r="G14" t="str">
+      <c r="G16" t="str">
         <v>skill:70040001</v>
       </c>
-      <c r="H14" t="str">
-        <v>护盾:+60|反射:15%</v>
-      </c>
-      <c r="I14" t="str">
+      <c r="H16" t="str">
+        <v>split:+1|splitAngle:+4|pierce:+1</v>
+      </c>
+      <c r="I16" t="str">
         <v>level:8</v>
       </c>
-      <c r="J14" t="str">
-        <v>护盾容量增加并反射部分激光。</v>
-      </c>
-      <c r="K14" t="str">
-        <v>icons/skill/seraphic_shell.png</v>
+      <c r="J16" t="str">
+        <v>精铸枪管令术弹再次分裂并保持贯穿。</v>
+      </c>
+      <c r="K16" t="str">
+        <v>icons/skill/riptide_collapse.png</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>70</v>
+      </c>
+      <c r="B17" t="str">
+        <v>04</v>
+      </c>
+      <c r="C17" t="str">
+        <v>0003</v>
+      </c>
+      <c r="D17" t="str">
+        <v>秘火迸流</v>
+      </c>
+      <c r="E17" t="str">
+        <v>工坊</v>
+      </c>
+      <c r="F17" t="str">
+        <v>3</v>
+      </c>
+      <c r="G17" t="str">
+        <v>skill:70040002</v>
+      </c>
+      <c r="H17" t="str">
+        <v>damageMultiplier:+12|luckBonus:+12|projectileSpeed:+16</v>
+      </c>
+      <c r="I17" t="str">
+        <v>level:11</v>
+      </c>
+      <c r="J17" t="str">
+        <v>秘火符文强化弹速与掉落运势。</v>
+      </c>
+      <c r="K17" t="str">
+        <v>icons/skill/choir_surge.png</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A4:K14"/>
+    <ignoredError numberStoredAsText="1" sqref="A4:K17"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>